<commit_message>
edited valuesets, readme, added path for current build in package-list.json
</commit_message>
<xml_diff>
--- a/build/website/StructureDefinition-cibmtr-observation-lab.xlsx
+++ b/build/website/StructureDefinition-cibmtr-observation-lab.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AP$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AP$60</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2992" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2296" uniqueCount="483">
   <si>
     <t>Path</t>
   </si>
@@ -1536,106 +1536,6 @@
   </si>
   <si>
     <t>outBoundRelationship[typeCode=COMP]</t>
-  </si>
-  <si>
-    <t>Observation.component.id</t>
-  </si>
-  <si>
-    <t>Observation.component.extension</t>
-  </si>
-  <si>
-    <t>Observation.component.modifierExtension</t>
-  </si>
-  <si>
-    <t>Observation.component.code</t>
-  </si>
-  <si>
-    <t>Type of component observation (code / type)</t>
-  </si>
-  <si>
-    <t>Describes what was observed. Sometimes this is called the observation "code".</t>
-  </si>
-  <si>
-    <t>*All* code-value and  component.code-component.value pairs need to be taken into account to correctly understand the meaning of the observation.</t>
-  </si>
-  <si>
-    <t>Codes identifying names of simple observations.</t>
-  </si>
-  <si>
-    <t>&lt; 363787002 |Observable entity| OR -&lt; 386053000 |Evaluation procedure|</t>
-  </si>
-  <si>
-    <t>Observation.component.value[x]</t>
-  </si>
-  <si>
-    <t>Actual component result</t>
-  </si>
-  <si>
-    <t>The information determined as a result of making the observation, if the information has a simple value.</t>
-  </si>
-  <si>
-    <t>Used when observation has a set of component observations. An observation may have both a value (e.g. an  Apgar score)  and component observations (the observations from which the Apgar score was derived). If a value is present, the datatype for this element should be determined by Observation.code. A CodeableConcept with just a text would be used instead of a string if the field was usually coded, or if the type associated with the Observation.code defines a coded value.  For additional guidance, see the [Notes section](http://hl7.org/fhir/R4/observation.html#notes) below.</t>
-  </si>
-  <si>
-    <t>363714003 |Interprets| &lt; 441742003 |Evaluation finding|</t>
-  </si>
-  <si>
-    <t>Observation.component.dataAbsentReason</t>
-  </si>
-  <si>
-    <t>Why the component result is missing</t>
-  </si>
-  <si>
-    <t>Provides a reason why the expected value in the element Observation.component.value[x] is missing.</t>
-  </si>
-  <si>
-    <t>"Null" or exceptional values can be represented two ways in FHIR Observations.  One way is to simply include them in the value set and represent the exceptions in the value.  For example, measurement values for a serology test could be  "detected", "not detected", "inconclusive", or  "test not done". 
-The alternate way is to use the value element for actual observations and use the explicit dataAbsentReason element to record exceptional values.  For example, the dataAbsentReason code "error" could be used when the measurement was not completed.  Because of these options, use-case agreements are required to interpret general observations for exceptional values.</t>
-  </si>
-  <si>
-    <t>Codes specifying why the result (`Observation.value[x]`) is missing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obs-6
-</t>
-  </si>
-  <si>
-    <t>Observation.component.interpretation</t>
-  </si>
-  <si>
-    <t>Observation.component.referenceRange</t>
-  </si>
-  <si>
-    <t>Provides guide for interpretation of component result</t>
-  </si>
-  <si>
-    <t>Guidance on how to interpret the value by comparison to a normal or recommended range.</t>
-  </si>
-  <si>
-    <t>GVHD</t>
-  </si>
-  <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="http://cdebrowser.nci.nih.gov"/&gt;
-    &lt;code value="3005293"/&gt;
-    &lt;display value="Type of Graft vs Host Disease (GVHD)"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>valueCodeableConcept</t>
-  </si>
-  <si>
-    <t>http://fhir.nmdp.org/ig/cibmtr-reporting/ValueSet/gvhdtype-valueset</t>
   </si>
 </sst>
 </file>
@@ -1784,7 +1684,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP78"/>
+  <dimension ref="A1:AP60"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1794,7 +1694,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="43.60546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.640625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.57421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
@@ -1817,13 +1717,13 @@
     <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.77734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="63.7421875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="50.89453125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.09765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="31" max="31" width="35.85546875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="26.328125" customWidth="true" bestFit="true"/>
@@ -9069,2192 +8969,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" hidden="true">
-      <c r="A61" t="s" s="2">
-        <v>483</v>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D61" s="2"/>
-      <c r="E61" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F61" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="J61" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="K61" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="M61" s="2"/>
-      <c r="N61" s="2"/>
-      <c r="O61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P61" s="2"/>
-      <c r="Q61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE61" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AF61" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG61" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AN61" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AO61" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP61" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="62" hidden="true">
-      <c r="A62" t="s" s="2">
-        <v>484</v>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="C62" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="D62" s="2"/>
-      <c r="E62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F62" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="G62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="J62" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="N62" s="2"/>
-      <c r="O62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P62" s="2"/>
-      <c r="Q62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE62" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AF62" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG62" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI62" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AJ62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AN62" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AO62" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP62" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="63" hidden="true">
-      <c r="A63" t="s" s="2">
-        <v>485</v>
-      </c>
-      <c r="B63" s="2"/>
-      <c r="C63" t="s" s="2">
-        <v>420</v>
-      </c>
-      <c r="D63" s="2"/>
-      <c r="E63" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F63" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="G63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H63" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="I63" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="J63" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K63" t="s" s="2">
-        <v>421</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="N63" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="O63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P63" s="2"/>
-      <c r="Q63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE63" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="AF63" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG63" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI63" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AJ63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AN63" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="AO63" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP63" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="64" hidden="true">
-      <c r="A64" t="s" s="2">
-        <v>486</v>
-      </c>
-      <c r="B64" s="2"/>
-      <c r="C64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D64" s="2"/>
-      <c r="E64" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="F64" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I64" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="J64" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="K64" t="s" s="2">
-        <v>487</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>488</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="O64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P64" s="2"/>
-      <c r="Q64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W64" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="X64" t="s" s="2">
-        <v>490</v>
-      </c>
-      <c r="Y64" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="Z64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE64" t="s" s="2">
-        <v>486</v>
-      </c>
-      <c r="AF64" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AG64" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI64" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK64" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL64" t="s" s="2">
-        <v>491</v>
-      </c>
-      <c r="AM64" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="AN64" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="AO64" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="AP64" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="65" hidden="true">
-      <c r="A65" t="s" s="2">
-        <v>492</v>
-      </c>
-      <c r="B65" s="2"/>
-      <c r="C65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D65" s="2"/>
-      <c r="E65" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F65" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I65" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="J65" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="K65" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>494</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>495</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="O65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P65" s="2"/>
-      <c r="Q65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE65" t="s" s="2">
-        <v>492</v>
-      </c>
-      <c r="AF65" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG65" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI65" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL65" t="s" s="2">
-        <v>496</v>
-      </c>
-      <c r="AM65" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="AN65" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="AO65" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP65" t="s" s="2">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="66" hidden="true">
-      <c r="A66" t="s" s="2">
-        <v>497</v>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D66" s="2"/>
-      <c r="E66" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F66" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="J66" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="K66" t="s" s="2">
-        <v>498</v>
-      </c>
-      <c r="L66" t="s" s="2">
-        <v>499</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>500</v>
-      </c>
-      <c r="N66" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="O66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P66" s="2"/>
-      <c r="Q66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W66" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="X66" t="s" s="2">
-        <v>501</v>
-      </c>
-      <c r="Y66" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="Z66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE66" t="s" s="2">
-        <v>497</v>
-      </c>
-      <c r="AF66" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG66" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH66" t="s" s="2">
-        <v>502</v>
-      </c>
-      <c r="AI66" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM66" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="AN66" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="AO66" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP66" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="67" hidden="true">
-      <c r="A67" t="s" s="2">
-        <v>503</v>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="D67" s="2"/>
-      <c r="E67" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="G67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="J67" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="K67" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="O67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P67" s="2"/>
-      <c r="Q67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W67" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="X67" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="Y67" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="Z67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE67" t="s" s="2">
-        <v>503</v>
-      </c>
-      <c r="AF67" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG67" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI67" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL67" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="AM67" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="AN67" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="AO67" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP67" t="s" s="2">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="68" hidden="true">
-      <c r="A68" t="s" s="2">
-        <v>504</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D68" s="2"/>
-      <c r="E68" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="G68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="J68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="K68" t="s" s="2">
-        <v>505</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>506</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="N68" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="O68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P68" s="2"/>
-      <c r="Q68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE68" t="s" s="2">
-        <v>504</v>
-      </c>
-      <c r="AF68" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI68" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="AN68" t="s" s="2">
-        <v>416</v>
-      </c>
-      <c r="AO68" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP68" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="69" hidden="true">
-      <c r="A69" t="s" s="2">
-        <v>474</v>
-      </c>
-      <c r="B69" t="s" s="2">
-        <v>507</v>
-      </c>
-      <c r="C69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D69" s="2"/>
-      <c r="E69" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F69" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I69" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="J69" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="K69" t="s" s="2">
-        <v>475</v>
-      </c>
-      <c r="L69" t="s" s="2">
-        <v>476</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>477</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>478</v>
-      </c>
-      <c r="O69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P69" s="2"/>
-      <c r="Q69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE69" t="s" s="2">
-        <v>474</v>
-      </c>
-      <c r="AF69" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI69" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM69" t="s" s="2">
-        <v>481</v>
-      </c>
-      <c r="AN69" t="s" s="2">
-        <v>482</v>
-      </c>
-      <c r="AO69" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP69" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="70" hidden="true">
-      <c r="A70" t="s" s="2">
-        <v>483</v>
-      </c>
-      <c r="B70" s="2"/>
-      <c r="C70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D70" s="2"/>
-      <c r="E70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F70" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="J70" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="K70" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
-      <c r="O70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P70" s="2"/>
-      <c r="Q70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE70" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AF70" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG70" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AJ70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AN70" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AO70" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP70" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="71" hidden="true">
-      <c r="A71" t="s" s="2">
-        <v>484</v>
-      </c>
-      <c r="B71" s="2"/>
-      <c r="C71" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="D71" s="2"/>
-      <c r="E71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="G71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="J71" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="L71" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="N71" s="2"/>
-      <c r="O71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P71" s="2"/>
-      <c r="Q71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE71" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AF71" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI71" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AJ71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AN71" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AO71" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP71" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="72" hidden="true">
-      <c r="A72" t="s" s="2">
-        <v>485</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" t="s" s="2">
-        <v>420</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="G72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H72" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="I72" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="J72" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="K72" t="s" s="2">
-        <v>421</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="N72" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="O72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P72" s="2"/>
-      <c r="Q72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="AF72" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI72" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AJ72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AN72" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="AO72" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP72" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="73" hidden="true">
-      <c r="A73" t="s" s="2">
-        <v>486</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D73" s="2"/>
-      <c r="E73" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="F73" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I73" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="J73" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="K73" t="s" s="2">
-        <v>487</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>488</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>489</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="O73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P73" s="2"/>
-      <c r="Q73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R73" t="s" s="2">
-        <v>508</v>
-      </c>
-      <c r="S73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W73" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="X73" t="s" s="2">
-        <v>490</v>
-      </c>
-      <c r="Y73" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="Z73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE73" t="s" s="2">
-        <v>486</v>
-      </c>
-      <c r="AF73" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AG73" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI73" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK73" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL73" t="s" s="2">
-        <v>491</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="AN73" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="AO73" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="AP73" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" hidden="true">
-      <c r="A74" t="s" s="2">
-        <v>492</v>
-      </c>
-      <c r="B74" s="2"/>
-      <c r="C74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F74" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I74" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="J74" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="K74" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>494</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>495</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="O74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P74" s="2"/>
-      <c r="Q74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA74" t="s" s="2">
-        <v>509</v>
-      </c>
-      <c r="AB74" s="2"/>
-      <c r="AC74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD74" t="s" s="2">
-        <v>510</v>
-      </c>
-      <c r="AE74" t="s" s="2">
-        <v>492</v>
-      </c>
-      <c r="AF74" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG74" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL74" t="s" s="2">
-        <v>496</v>
-      </c>
-      <c r="AM74" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="AN74" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="AO74" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP74" t="s" s="2">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="75" hidden="true">
-      <c r="A75" t="s" s="2">
-        <v>492</v>
-      </c>
-      <c r="B75" t="s" s="2">
-        <v>511</v>
-      </c>
-      <c r="C75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D75" s="2"/>
-      <c r="E75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F75" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I75" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="J75" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="K75" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>494</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>495</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="O75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P75" s="2"/>
-      <c r="Q75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W75" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="X75" s="2"/>
-      <c r="Y75" t="s" s="2">
-        <v>512</v>
-      </c>
-      <c r="Z75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE75" t="s" s="2">
-        <v>492</v>
-      </c>
-      <c r="AF75" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG75" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI75" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL75" t="s" s="2">
-        <v>496</v>
-      </c>
-      <c r="AM75" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="AN75" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="AO75" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP75" t="s" s="2">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="76" hidden="true">
-      <c r="A76" t="s" s="2">
-        <v>497</v>
-      </c>
-      <c r="B76" s="2"/>
-      <c r="C76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D76" s="2"/>
-      <c r="E76" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F76" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="G76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="J76" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="K76" t="s" s="2">
-        <v>498</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>499</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>500</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="O76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P76" s="2"/>
-      <c r="Q76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W76" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="X76" t="s" s="2">
-        <v>501</v>
-      </c>
-      <c r="Y76" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="Z76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE76" t="s" s="2">
-        <v>497</v>
-      </c>
-      <c r="AF76" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG76" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH76" t="s" s="2">
-        <v>502</v>
-      </c>
-      <c r="AI76" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM76" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="AN76" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="AO76" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP76" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="77" hidden="true">
-      <c r="A77" t="s" s="2">
-        <v>503</v>
-      </c>
-      <c r="B77" s="2"/>
-      <c r="C77" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="D77" s="2"/>
-      <c r="E77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F77" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="G77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="J77" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="K77" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="N77" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="O77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P77" s="2"/>
-      <c r="Q77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W77" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="X77" t="s" s="2">
-        <v>357</v>
-      </c>
-      <c r="Y77" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="Z77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE77" t="s" s="2">
-        <v>503</v>
-      </c>
-      <c r="AF77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG77" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI77" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL77" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="AM77" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="AN77" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="AO77" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP77" t="s" s="2">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="78" hidden="true">
-      <c r="A78" t="s" s="2">
-        <v>504</v>
-      </c>
-      <c r="B78" s="2"/>
-      <c r="C78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D78" s="2"/>
-      <c r="E78" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="F78" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="G78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="H78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="I78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="J78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="K78" t="s" s="2">
-        <v>505</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>506</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="N78" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="O78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="P78" s="2"/>
-      <c r="Q78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="R78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="S78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="T78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="U78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="V78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="W78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="X78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Y78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="Z78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AA78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AB78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AC78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AD78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AE78" t="s" s="2">
-        <v>504</v>
-      </c>
-      <c r="AF78" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AG78" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AH78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AI78" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AJ78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AK78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AL78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AM78" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="AN78" t="s" s="2">
-        <v>416</v>
-      </c>
-      <c r="AO78" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="AP78" t="s" s="2">
-        <v>46</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AP78">
+  <autoFilter ref="A1:AP60">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -11264,7 +8980,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI77">
+  <conditionalFormatting sqref="A2:AI59">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>